<commit_message>
MOD: Actualizado notas pendientes
</commit_message>
<xml_diff>
--- a/NotasAcumuladasFaltaProyecto3.xlsx
+++ b/NotasAcumuladasFaltaProyecto3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\GIT\POO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A0262F-D54B-4553-B07C-997AED361BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D53F88B-C96E-4CA6-B0F0-A42624703E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20280" yWindow="-2940" windowWidth="29040" windowHeight="15840" xr2:uid="{DADB371E-097B-40F2-82D5-B24D16BBBB40}"/>
   </bookViews>
@@ -40,7 +40,6 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={F5B8D2A8-63BA-4101-836C-1635D4E40C86}</author>
-    <author>tc={76533352-217C-4B79-9964-18108F7C5CDC}</author>
   </authors>
   <commentList>
     <comment ref="I9" authorId="0" shapeId="0" xr:uid="{F5B8D2A8-63BA-4101-836C-1635D4E40C86}">
@@ -49,14 +48,6 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Tiene un fork de mi repo. Revisar</t>
-      </text>
-    </comment>
-    <comment ref="J11" authorId="1" shapeId="0" xr:uid="{76533352-217C-4B79-9964-18108F7C5CDC}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    No me carga la URL</t>
       </text>
     </comment>
   </commentList>
@@ -529,12 +520,12 @@
       <sheetData sheetId="5">
         <row r="26">
           <cell r="K26">
-            <v>3.7</v>
+            <v>3.6</v>
           </cell>
         </row>
         <row r="27">
           <cell r="K27">
-            <v>3.6</v>
+            <v>3.9</v>
           </cell>
         </row>
         <row r="28">
@@ -549,7 +540,7 @@
         </row>
         <row r="30">
           <cell r="K30">
-            <v>4</v>
+            <v>3.8</v>
           </cell>
         </row>
         <row r="31">
@@ -559,22 +550,22 @@
         </row>
         <row r="32">
           <cell r="K32">
-            <v>3.7</v>
+            <v>3.8</v>
           </cell>
         </row>
         <row r="33">
           <cell r="K33">
-            <v>4.3</v>
+            <v>4.2</v>
           </cell>
         </row>
         <row r="34">
           <cell r="K34">
-            <v>4</v>
+            <v>3.9</v>
           </cell>
         </row>
         <row r="35">
           <cell r="K35">
-            <v>4.4000000000000004</v>
+            <v>4.3</v>
           </cell>
         </row>
         <row r="36">
@@ -589,7 +580,7 @@
         </row>
         <row r="38">
           <cell r="K38">
-            <v>3.9</v>
+            <v>3.7</v>
           </cell>
         </row>
         <row r="39">
@@ -604,12 +595,12 @@
         </row>
         <row r="41">
           <cell r="K41">
-            <v>4.0999999999999996</v>
+            <v>4.2</v>
           </cell>
         </row>
         <row r="42">
           <cell r="K42">
-            <v>4.2</v>
+            <v>4.0999999999999996</v>
           </cell>
         </row>
       </sheetData>
@@ -1194,9 +1185,6 @@
   <threadedComment ref="I9" dT="2021-10-06T21:48:46.63" personId="{00000000-0000-0000-0000-000000000000}" id="{F5B8D2A8-63BA-4101-836C-1635D4E40C86}">
     <text>Tiene un fork de mi repo. Revisar</text>
   </threadedComment>
-  <threadedComment ref="J11" dT="2021-10-06T21:54:58.52" personId="{00000000-0000-0000-0000-000000000000}" id="{76533352-217C-4B79-9964-18108F7C5CDC}">
-    <text>No me carga la URL</text>
-  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1204,13 +1192,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABAD6323-CDD4-415B-86AC-36AAC5EBE687}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="8" width="14.5703125" customWidth="1"/>
     <col min="9" max="15" width="19.140625" customWidth="1"/>
     <col min="16" max="16" width="9.140625" style="17"/>
@@ -1312,7 +1300,7 @@
       </c>
       <c r="E3" s="7">
         <f>ROUND([1]Parcial!K26,1)</f>
-        <v>3.7</v>
+        <v>3.6</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7">
@@ -1321,7 +1309,7 @@
       </c>
       <c r="H3" s="11">
         <f>ROUND(AVERAGE(I3:O3),1)</f>
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="I3" s="12">
         <v>5</v>
@@ -1337,7 +1325,7 @@
         <v>5</v>
       </c>
       <c r="M3" s="13">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="N3" s="13">
         <v>0</v>
@@ -1348,7 +1336,7 @@
       </c>
       <c r="P3" s="16">
         <f>D3*$D$1+E3*$E$1+H3*$H$1+G3*$G$1+F3*$F$1</f>
-        <v>2.2800000000000002</v>
+        <v>2.4400000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="51">
@@ -1367,7 +1355,7 @@
       </c>
       <c r="E4" s="7">
         <f>ROUND([1]Parcial!K27,1)</f>
-        <v>3.6</v>
+        <v>3.9</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7">
@@ -1403,7 +1391,7 @@
       </c>
       <c r="P4" s="16">
         <f>D4*$D$1+E4*$E$1+H4*$H$1+G4*$G$1+F4*$F$1</f>
-        <v>3.5</v>
+        <v>3.56</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="63.75">
@@ -1532,7 +1520,7 @@
       </c>
       <c r="E7" s="7">
         <f>ROUND([1]Parcial!K30,1)</f>
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7">
@@ -1568,7 +1556,7 @@
       </c>
       <c r="P7" s="16">
         <f>D7*$D$1+E7*$E$1+H7*$H$1+G7*$G$1+F7*$F$1</f>
-        <v>2.73</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="38.25">
@@ -1642,7 +1630,7 @@
       </c>
       <c r="E9" s="7">
         <f>ROUND([1]Parcial!K32,1)</f>
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7">
@@ -1678,7 +1666,7 @@
       </c>
       <c r="P9" s="16">
         <f>D9*$D$1+E9*$E$1+H9*$H$1+G9*$G$1+F9*$F$1</f>
-        <v>2.62</v>
+        <v>2.64</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="51">
@@ -1697,7 +1685,7 @@
       </c>
       <c r="E10" s="7">
         <f>ROUND([1]Parcial!K33,1)</f>
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7">
@@ -1733,7 +1721,7 @@
       </c>
       <c r="P10" s="16">
         <f>D10*$D$1+E10*$E$1+H10*$H$1+G10*$G$1+F10*$F$1</f>
-        <v>3.5100000000000002</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="38.25">
@@ -1752,7 +1740,7 @@
       </c>
       <c r="E11" s="7">
         <f>ROUND([1]Parcial!K34,1)</f>
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7">
@@ -1761,13 +1749,13 @@
       </c>
       <c r="H11" s="11">
         <f>ROUND(AVERAGE(I11:O11),1)</f>
-        <v>4.0999999999999996</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I11" s="12">
         <v>5</v>
       </c>
       <c r="J11" s="12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K11" s="12">
         <f>[1]TareaDebugger!K11</f>
@@ -1788,7 +1776,7 @@
       </c>
       <c r="P11" s="16">
         <f>D11*$D$1+E11*$E$1+H11*$H$1+G11*$G$1+F11*$F$1</f>
-        <v>3.18</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="51">
@@ -1807,7 +1795,7 @@
       </c>
       <c r="E12" s="7">
         <f>ROUND([1]Parcial!K35,1)</f>
-        <v>4.4000000000000004</v>
+        <v>4.3</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7">
@@ -1843,7 +1831,7 @@
       </c>
       <c r="P12" s="16">
         <f>D12*$D$1+E12*$E$1+H12*$H$1+G12*$G$1+F12*$F$1</f>
-        <v>1.68</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="51">
@@ -1972,7 +1960,7 @@
       </c>
       <c r="E15" s="7">
         <f>ROUND([1]Parcial!K38,1)</f>
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7">
@@ -2008,7 +1996,7 @@
       </c>
       <c r="P15" s="16">
         <f>D15*$D$1+E15*$E$1+H15*$H$1+G15*$G$1+F15*$F$1</f>
-        <v>3.16</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="51">
@@ -2137,7 +2125,7 @@
       </c>
       <c r="E18" s="7">
         <f>ROUND([1]Parcial!K41,1)</f>
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7">
@@ -2173,7 +2161,7 @@
       </c>
       <c r="P18" s="16">
         <f>D18*$D$1+E18*$E$1+H18*$H$1+G18*$G$1+F18*$F$1</f>
-        <v>2.9</v>
+        <v>2.9200000000000004</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="38.25">
@@ -2192,7 +2180,7 @@
       </c>
       <c r="E19" s="7">
         <f>ROUND([1]Parcial!K42,1)</f>
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7">
@@ -2228,7 +2216,7 @@
       </c>
       <c r="P19" s="16">
         <f>D19*$D$1+E19*$E$1+H19*$H$1+G19*$G$1+F19*$F$1</f>
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>